<commit_message>
Implemented stack using linkedlist in java
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GT\DSA_ZTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7204FAB-04E1-4089-9C57-4CA81FE0C3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76331A4-8B2D-442C-B587-1A660F206C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="466">
   <si>
     <t>Topic:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>&lt;yes&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Yes&gt;</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3300,7 +3303,7 @@
         <v>134</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">

</xml_diff>